<commit_message>
Actualizacion entradas y comiendo con lectura de datos.
</commit_message>
<xml_diff>
--- a/entrada/Canarias/SectoresNucleos_Canarias.xlsx
+++ b/entrada/Canarias/SectoresNucleos_Canarias.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aperillo\Documents\ABACO\Datos de entorno\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tinot\eclipse-workspace\Proyecto-Salomon\entrada\Canarias\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8945503-D1F7-4570-8C14-EA414AA2A96F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -125,13 +126,13 @@
     <t>RUTA</t>
   </si>
   <si>
-    <t>Canarias Ruta</t>
+    <t>Ruta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -445,26 +446,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="2" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -472,7 +473,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -483,7 +484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -494,7 +495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -505,7 +506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -516,7 +517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -527,7 +528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -538,7 +539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -549,7 +550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -560,7 +561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
@@ -571,7 +572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -582,7 +583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -593,7 +594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -604,7 +605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
@@ -615,7 +616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
@@ -626,7 +627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
@@ -637,7 +638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
@@ -648,7 +649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
@@ -659,7 +660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>11</v>
       </c>
@@ -670,7 +671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
@@ -681,7 +682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>12</v>
       </c>
@@ -692,7 +693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>6</v>
       </c>
@@ -703,7 +704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
@@ -714,7 +715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
@@ -725,7 +726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>13</v>
       </c>
@@ -736,7 +737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
@@ -747,7 +748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>14</v>
       </c>
@@ -758,7 +759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
@@ -769,7 +770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>3</v>
       </c>
@@ -780,7 +781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
@@ -791,7 +792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>12</v>
       </c>
@@ -802,7 +803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>10</v>
       </c>
@@ -813,7 +814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>7</v>
       </c>
@@ -824,7 +825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>13</v>
       </c>
@@ -835,7 +836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>12</v>
       </c>
@@ -846,7 +847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>2</v>
       </c>
@@ -857,7 +858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>13</v>
       </c>
@@ -868,7 +869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>15</v>
       </c>
@@ -879,7 +880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>10</v>
       </c>
@@ -890,7 +891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>2</v>
       </c>
@@ -901,7 +902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>16</v>
       </c>
@@ -912,7 +913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>17</v>
       </c>
@@ -923,7 +924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>18</v>
       </c>
@@ -934,7 +935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>19</v>
       </c>
@@ -945,7 +946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>20</v>
       </c>
@@ -956,7 +957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>17</v>
       </c>
@@ -967,7 +968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>19</v>
       </c>
@@ -978,7 +979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>16</v>
       </c>
@@ -989,7 +990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>21</v>
       </c>
@@ -1000,7 +1001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>22</v>
       </c>
@@ -1011,7 +1012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>23</v>
       </c>
@@ -1022,7 +1023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>24</v>
       </c>
@@ -1033,7 +1034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>19</v>
       </c>
@@ -1044,7 +1045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>25</v>
       </c>
@@ -1055,7 +1056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>19</v>
       </c>
@@ -1066,7 +1067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>22</v>
       </c>
@@ -1077,7 +1078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>21</v>
       </c>
@@ -1088,7 +1089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>26</v>
       </c>
@@ -1099,7 +1100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>27</v>
       </c>
@@ -1110,7 +1111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>19</v>
       </c>
@@ -1121,7 +1122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>28</v>
       </c>
@@ -1132,7 +1133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>19</v>
       </c>
@@ -1143,7 +1144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>26</v>
       </c>
@@ -1154,7 +1155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>18</v>
       </c>
@@ -1165,7 +1166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>20</v>
       </c>
@@ -1176,7 +1177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>24</v>
       </c>
@@ -1187,7 +1188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>19</v>
       </c>
@@ -1198,7 +1199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>26</v>
       </c>
@@ -1209,7 +1210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>21</v>
       </c>
@@ -1220,7 +1221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>23</v>
       </c>
@@ -1231,7 +1232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>22</v>
       </c>
@@ -1242,7 +1243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>19</v>
       </c>
@@ -1253,7 +1254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>25</v>
       </c>
@@ -1264,7 +1265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>17</v>
       </c>
@@ -1275,7 +1276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>19</v>
       </c>
@@ -1286,7 +1287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>24</v>
       </c>
@@ -1297,7 +1298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>16</v>
       </c>
@@ -1308,7 +1309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>19</v>
       </c>
@@ -1319,7 +1320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>20</v>
       </c>
@@ -1330,7 +1331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>18</v>
       </c>
@@ -1341,7 +1342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>25</v>
       </c>
@@ -1352,7 +1353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>23</v>
       </c>
@@ -1363,7 +1364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>29</v>
       </c>
@@ -1374,7 +1375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>3</v>
       </c>
@@ -1385,7 +1386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>10</v>
       </c>
@@ -1396,7 +1397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>2</v>
       </c>
@@ -1407,7 +1408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>15</v>
       </c>
@@ -1418,7 +1419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>29</v>
       </c>
@@ -1429,7 +1430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>3</v>
       </c>
@@ -1440,7 +1441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>2</v>
       </c>
@@ -1451,7 +1452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>12</v>
       </c>
@@ -1462,7 +1463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>7</v>
       </c>
@@ -1473,7 +1474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>3</v>
       </c>
@@ -1484,7 +1485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>29</v>
       </c>
@@ -1495,7 +1496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>2</v>
       </c>
@@ -1506,7 +1507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>14</v>
       </c>
@@ -1517,7 +1518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>2</v>
       </c>
@@ -1528,7 +1529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>11</v>
       </c>
@@ -1539,7 +1540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>10</v>
       </c>
@@ -1550,7 +1551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>12</v>
       </c>
@@ -1561,7 +1562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>29</v>
       </c>
@@ -1572,7 +1573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>30</v>
       </c>
@@ -1583,7 +1584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>30</v>
       </c>

</xml_diff>